<commit_message>
first 2 rules of LL grammar implemented, improvements in LL grammar
</commit_message>
<xml_diff>
--- a/LL_Grammar.xlsx
+++ b/LL_Grammar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vutbr-my.sharepoint.com/personal/xhruzt00_vutbr_cz/Documents/Dokumenty/FIT/5_semester/IFJ/projektNew/IFJ20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="114_{2A041381-6877-43E3-8854-82C133F41085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{898B2952-4B4E-43CD-92C0-D6362B3A3CF1}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="114_{2A041381-6877-43E3-8854-82C133F41085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{063277A3-F22F-443D-AD44-2728309C2623}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="48">
   <si>
     <t>&lt;prolog&gt;</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>&lt;stat_list&gt;</t>
-  </si>
-  <si>
-    <t>&lt;main_fun&gt;</t>
   </si>
   <si>
     <t>func</t>
@@ -548,13 +545,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>46829</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>94643</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -854,24 +851,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="13" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="13" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>0</v>
@@ -880,14 +877,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="29" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="29"/>
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
@@ -895,15 +888,15 @@
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>6</v>
@@ -918,7 +911,7 @@
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -926,7 +919,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>1</v>
@@ -941,93 +934,107 @@
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+        <v>8</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>1</v>
+      </c>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>
       <c r="M4" s="29"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="29" t="s">
+      <c r="B6" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="F6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="G6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="H6" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="I6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="J6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="29" t="s">
+      <c r="K6" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="29"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="29" t="s">
+      <c r="M6" s="29"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="29"/>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
@@ -1039,19 +1046,15 @@
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>22</v>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>22</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
@@ -1062,15 +1065,19 @@
       <c r="L8" s="29"/>
       <c r="M8" s="29"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
@@ -1081,16 +1088,14 @@
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>24</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
@@ -1102,14 +1107,16 @@
       <c r="L10" s="29"/>
       <c r="M10" s="29"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>24</v>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="29"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
@@ -1121,12 +1128,12 @@
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -1140,12 +1147,12 @@
       <c r="L12" s="29"/>
       <c r="M12" s="29"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>26</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
@@ -1159,16 +1166,14 @@
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>15</v>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>29</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
@@ -1180,15 +1185,15 @@
       <c r="L14" s="29"/>
       <c r="M14" s="29"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
@@ -1201,19 +1206,17 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>29</v>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>29</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D16" s="29"/>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
@@ -1224,15 +1227,19 @@
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+        <v>26</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>28</v>
+      </c>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
@@ -1243,12 +1250,12 @@
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
@@ -1262,22 +1269,16 @@
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>7</v>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>7</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
       <c r="H19" s="29"/>
@@ -1287,16 +1288,22 @@
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
       <c r="H20" s="29"/>
@@ -1306,107 +1313,105 @@
       <c r="L20" s="29"/>
       <c r="M20" s="29"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>30</v>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>17</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
       <c r="M21" s="29"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="29" t="s">
-        <v>32</v>
-      </c>
       <c r="C22" s="29" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E22" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>41</v>
-      </c>
       <c r="H22" s="29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I22" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J22" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="K22" s="29" t="s">
-        <v>17</v>
-      </c>
+      <c r="K22" s="29"/>
       <c r="L22" s="29"/>
       <c r="M22" s="29"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
+        <v>31</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>16</v>
+      </c>
       <c r="L23" s="29"/>
       <c r="M23" s="29"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>44</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C24" s="29"/>
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
       <c r="F24" s="29"/>
@@ -1418,14 +1423,16 @@
       <c r="L24" s="29"/>
       <c r="M24" s="29"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="29"/>
+        <v>32</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
@@ -1437,12 +1444,12 @@
       <c r="L25" s="29"/>
       <c r="M25" s="29"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
@@ -1456,22 +1463,16 @@
       <c r="L26" s="29"/>
       <c r="M26" s="29"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>42</v>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>6</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
@@ -1481,16 +1482,22 @@
       <c r="L27" s="29"/>
       <c r="M27" s="29"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
+        <v>41</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>6</v>
+      </c>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
       <c r="H28" s="29"/>
@@ -1500,22 +1507,16 @@
       <c r="L28" s="29"/>
       <c r="M28" s="29"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>6</v>
-      </c>
+      <c r="B29" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
@@ -1525,16 +1526,22 @@
       <c r="L29" s="29"/>
       <c r="M29" s="29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
+        <v>40</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>6</v>
+      </c>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
       <c r="H30" s="29"/>
@@ -1544,16 +1551,14 @@
       <c r="L30" s="29"/>
       <c r="M30" s="29"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>43</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C31" s="29"/>
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
@@ -1565,19 +1570,17 @@
       <c r="L31" s="29"/>
       <c r="M31" s="29"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D32" s="29"/>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
@@ -1588,15 +1591,19 @@
       <c r="L32" s="29"/>
       <c r="M32" s="29"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
+        <v>22</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>42</v>
+      </c>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
@@ -1607,16 +1614,14 @@
       <c r="L33" s="29"/>
       <c r="M33" s="29"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>44</v>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>44</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C34" s="29"/>
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
@@ -1628,19 +1633,17 @@
       <c r="L34" s="29"/>
       <c r="M34" s="29"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D35" s="29"/>
       <c r="E35" s="29"/>
       <c r="F35" s="29"/>
       <c r="G35" s="29"/>
@@ -1651,15 +1654,19 @@
       <c r="L35" s="29"/>
       <c r="M35" s="29"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
       <c r="E36" s="29"/>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
@@ -1670,12 +1677,12 @@
       <c r="L36" s="29"/>
       <c r="M36" s="29"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
@@ -1689,12 +1696,12 @@
       <c r="L37" s="29"/>
       <c r="M37" s="29"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>6</v>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
@@ -1708,14 +1715,16 @@
       <c r="L38" s="29"/>
       <c r="M38" s="29"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="29"/>
+        <v>6</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>18</v>
+      </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
       <c r="F39" s="29"/>
@@ -1727,22 +1736,16 @@
       <c r="L39" s="29"/>
       <c r="M39" s="29"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>14</v>
-      </c>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>
       <c r="H40" s="29"/>
@@ -1752,18 +1755,22 @@
       <c r="L40" s="29"/>
       <c r="M40" s="29"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
-        <v>45</v>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
+        <v>12</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>13</v>
+      </c>
       <c r="F41" s="29"/>
       <c r="G41" s="29"/>
       <c r="H41" s="29"/>
@@ -1773,19 +1780,17 @@
       <c r="L41" s="29"/>
       <c r="M41" s="29"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D42" s="29"/>
       <c r="E42" s="29"/>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
@@ -1796,75 +1801,67 @@
       <c r="L42" s="29"/>
       <c r="M42" s="29"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="33"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="17"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="25"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="34"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="17"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="20"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="23"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
@@ -1876,10 +1873,10 @@
       <c r="L46" s="22"/>
       <c r="M46" s="25"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="20"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
@@ -1891,38 +1888,53 @@
       <c r="L47" s="22"/>
       <c r="M47" s="25"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="27"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="20"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="25"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" s="21"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="27"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="24"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="24"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="22"/>
+      <c r="B54" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Syntax analysis almost done, few rules are missing
</commit_message>
<xml_diff>
--- a/LL_Grammar.xlsx
+++ b/LL_Grammar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vutbr-my.sharepoint.com/personal/xhruzt00_vutbr_cz/Documents/Dokumenty/FIT/5_semester/IFJ/projektNew/IFJ20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="114_{2A041381-6877-43E3-8854-82C133F41085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{063277A3-F22F-443D-AD44-2728309C2623}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="114_{2A041381-6877-43E3-8854-82C133F41085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6DE49F0D-0AC8-4F52-A4A4-3CBF13BB82B8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="49">
   <si>
     <t>&lt;prolog&gt;</t>
   </si>
@@ -36,9 +36,6 @@
     <t>&lt;prog&gt;</t>
   </si>
   <si>
-    <t>&lt;EOF&gt;</t>
-  </si>
-  <si>
     <t>&lt;fun_def&gt;</t>
   </si>
   <si>
@@ -169,6 +166,12 @@
   </si>
   <si>
     <t>Ako s EOL?</t>
+  </si>
+  <si>
+    <t>EOF</t>
+  </si>
+  <si>
+    <t>&lt;opt_exp&gt;</t>
   </si>
 </sst>
 </file>
@@ -191,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +288,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -520,6 +535,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -545,14 +575,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>46829</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>94643</xdr:rowOff>
+      <xdr:colOff>41114</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>109883</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -851,24 +881,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="13" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>0</v>
@@ -877,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
@@ -888,18 +918,18 @@
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
@@ -911,15 +941,15 @@
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>1</v>
@@ -934,106 +964,104 @@
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="29" t="s">
+      <c r="D5" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="29" t="s">
+      <c r="F5" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="29"/>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="F6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="G6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="H6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="I6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="J6" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="29" t="s">
+      <c r="K6" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="29" t="s">
-        <v>16</v>
-      </c>
       <c r="M6" s="29"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>21</v>
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
@@ -1046,12 +1074,12 @@
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -1065,18 +1093,18 @@
       <c r="L8" s="29"/>
       <c r="M8" s="29"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>20</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>21</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
@@ -1088,12 +1116,12 @@
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -1107,15 +1135,15 @@
       <c r="L10" s="29"/>
       <c r="M10" s="29"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
@@ -1128,12 +1156,12 @@
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -1147,12 +1175,12 @@
       <c r="L12" s="29"/>
       <c r="M12" s="29"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>24</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
@@ -1166,12 +1194,12 @@
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
@@ -1185,15 +1213,15 @@
       <c r="L14" s="29"/>
       <c r="M14" s="29"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>27</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>28</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
@@ -1206,15 +1234,15 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
@@ -1227,18 +1255,18 @@
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="D17" s="29" t="s">
         <v>27</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>28</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
@@ -1250,12 +1278,12 @@
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
@@ -1269,12 +1297,12 @@
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
@@ -1288,21 +1316,21 @@
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>6</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>7</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
@@ -1313,12 +1341,12 @@
       <c r="L20" s="29"/>
       <c r="M20" s="29"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -1332,84 +1360,86 @@
       <c r="L21" s="29"/>
       <c r="M21" s="29"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="29" t="s">
-        <v>30</v>
-      </c>
       <c r="C22" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="H22" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" s="29" t="s">
         <v>15</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="J22" s="29" t="s">
-        <v>16</v>
       </c>
       <c r="K22" s="29"/>
       <c r="L22" s="29"/>
       <c r="M22" s="29"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G23" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23" s="29"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>41</v>
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
@@ -1423,15 +1453,15 @@
       <c r="L24" s="29"/>
       <c r="M24" s="29"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
@@ -1444,12 +1474,12 @@
       <c r="L25" s="29"/>
       <c r="M25" s="29"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
@@ -1463,12 +1493,12 @@
       <c r="L26" s="29"/>
       <c r="M26" s="29"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
@@ -1482,22 +1512,20 @@
       <c r="L27" s="29"/>
       <c r="M27" s="29"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>6</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E28" s="29"/>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
       <c r="H28" s="29"/>
@@ -1507,12 +1535,12 @@
       <c r="L28" s="29"/>
       <c r="M28" s="29"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
@@ -1526,22 +1554,20 @@
       <c r="L29" s="29"/>
       <c r="M29" s="29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>40</v>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
+        <v>39</v>
       </c>
       <c r="B30" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>6</v>
-      </c>
+      <c r="E30" s="29"/>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
       <c r="H30" s="29"/>
@@ -1551,14 +1577,16 @@
       <c r="L30" s="29"/>
       <c r="M30" s="29"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>40</v>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="38" t="s">
+        <v>41</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="29"/>
+        <v>9</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>41</v>
+      </c>
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
@@ -1570,17 +1598,19 @@
       <c r="L31" s="29"/>
       <c r="M31" s="29"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
-        <v>42</v>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
+        <v>41</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="29"/>
+        <v>9</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>41</v>
+      </c>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
@@ -1591,19 +1621,15 @@
       <c r="L32" s="29"/>
       <c r="M32" s="29"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
-        <v>42</v>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="38" t="s">
+        <v>41</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>42</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
@@ -1614,14 +1640,16 @@
       <c r="L33" s="29"/>
       <c r="M33" s="29"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="29"/>
+        <v>34</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>42</v>
+      </c>
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
@@ -1633,17 +1661,19 @@
       <c r="L34" s="29"/>
       <c r="M34" s="29"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>43</v>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
+        <v>42</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="29"/>
+        <v>34</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>42</v>
+      </c>
       <c r="E35" s="29"/>
       <c r="F35" s="29"/>
       <c r="G35" s="29"/>
@@ -1654,19 +1684,15 @@
       <c r="L35" s="29"/>
       <c r="M35" s="29"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
-        <v>43</v>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="39" t="s">
+        <v>42</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>43</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="29"/>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
@@ -1677,12 +1703,12 @@
       <c r="L36" s="29"/>
       <c r="M36" s="29"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="30" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
         <v>42</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>32</v>
       </c>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
@@ -1696,12 +1722,12 @@
       <c r="L37" s="29"/>
       <c r="M37" s="29"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>43</v>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="37" t="s">
+        <v>48</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
@@ -1715,16 +1741,14 @@
       <c r="L38" s="29"/>
       <c r="M38" s="29"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>18</v>
-      </c>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="29"/>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
       <c r="F39" s="29"/>
@@ -1736,14 +1760,16 @@
       <c r="L39" s="29"/>
       <c r="M39" s="29"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="29"/>
+      <c r="C40" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
@@ -1755,22 +1781,16 @@
       <c r="L40" s="29"/>
       <c r="M40" s="29"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="29" t="s">
-        <v>13</v>
-      </c>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
       <c r="F41" s="29"/>
       <c r="G41" s="29"/>
       <c r="H41" s="29"/>
@@ -1780,18 +1800,22 @@
       <c r="L41" s="29"/>
       <c r="M41" s="29"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="s">
-        <v>44</v>
+    <row r="42" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
+        <v>11</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>12</v>
+      </c>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
       <c r="H42" s="29"/>
@@ -1801,19 +1825,17 @@
       <c r="L42" s="29"/>
       <c r="M42" s="29"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D43" s="29"/>
       <c r="E43" s="29"/>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
@@ -1824,59 +1846,67 @@
       <c r="L43" s="29"/>
       <c r="M43" s="29"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A45" s="34"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="17"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" s="20"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="25"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="34"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="29"/>
+      <c r="M46" s="17"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="20"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="23"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="22"/>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
@@ -1888,10 +1918,10 @@
       <c r="L47" s="22"/>
       <c r="M47" s="25"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="20"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="22"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="23"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
@@ -1903,38 +1933,53 @@
       <c r="L48" s="22"/>
       <c r="M48" s="25"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A49" s="21"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="27"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A52" s="19" t="s">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="25"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="27"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="24"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="24"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A53" s="28" t="s">
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54" s="22"/>
+      <c r="B55" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
parser, basic grammar done
</commit_message>
<xml_diff>
--- a/LL_Grammar.xlsx
+++ b/LL_Grammar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vutbr-my.sharepoint.com/personal/xhruzt00_vutbr_cz/Documents/Dokumenty/FIT/5_semester/IFJ/projektNew/IFJ20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="114_{2A041381-6877-43E3-8854-82C133F41085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6DE49F0D-0AC8-4F52-A4A4-3CBF13BB82B8}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="114_{2A041381-6877-43E3-8854-82C133F41085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F3DFE4E-A7F0-4F53-B816-6E160D2D246A}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="51">
   <si>
     <t>&lt;prolog&gt;</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>&lt;opt_exp&gt;</t>
+  </si>
+  <si>
+    <t>id + 5</t>
+  </si>
+  <si>
+    <t>asdasdsadsadasdasdasdsad + 5</t>
   </si>
 </sst>
 </file>
@@ -881,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,7 +1261,7 @@
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>27</v>
       </c>
@@ -1278,7 +1284,7 @@
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
@@ -1296,8 +1302,11 @@
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>26</v>
       </c>
@@ -1316,7 +1325,7 @@
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>6</v>
       </c>
@@ -1340,8 +1349,14 @@
       <c r="K20" s="29"/>
       <c r="L20" s="29"/>
       <c r="M20" s="29"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>6</v>
       </c>
@@ -1360,7 +1375,7 @@
       <c r="L21" s="29"/>
       <c r="M21" s="29"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
@@ -1395,7 +1410,7 @@
       <c r="L22" s="29"/>
       <c r="M22" s="29"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>28</v>
       </c>
@@ -1434,7 +1449,7 @@
       </c>
       <c r="M23" s="29"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>28</v>
       </c>
@@ -1453,7 +1468,7 @@
       <c r="L24" s="29"/>
       <c r="M24" s="29"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>28</v>
       </c>
@@ -1474,7 +1489,7 @@
       <c r="L25" s="29"/>
       <c r="M25" s="29"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>28</v>
       </c>
@@ -1493,7 +1508,7 @@
       <c r="L26" s="29"/>
       <c r="M26" s="29"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>28</v>
       </c>
@@ -1512,7 +1527,7 @@
       <c r="L27" s="29"/>
       <c r="M27" s="29"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>40</v>
       </c>
@@ -1535,7 +1550,7 @@
       <c r="L28" s="29"/>
       <c r="M28" s="29"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>40</v>
       </c>
@@ -1554,7 +1569,7 @@
       <c r="L29" s="29"/>
       <c r="M29" s="29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
         <v>39</v>
       </c>
@@ -1577,7 +1592,7 @@
       <c r="L30" s="29"/>
       <c r="M30" s="29"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="38" t="s">
         <v>41</v>
       </c>
@@ -1598,7 +1613,7 @@
       <c r="L31" s="29"/>
       <c r="M31" s="29"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
input,print functions; declarations in fun defs
</commit_message>
<xml_diff>
--- a/LL_Grammar.xlsx
+++ b/LL_Grammar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vutbr-my.sharepoint.com/personal/xhruzt00_vutbr_cz/Documents/Dokumenty/FIT/5_semester/IFJ/projektNew/IFJ20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="114_{2A041381-6877-43E3-8854-82C133F41085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F3DFE4E-A7F0-4F53-B816-6E160D2D246A}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="114_{2A041381-6877-43E3-8854-82C133F41085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E7750B61-D6CA-4282-8C7B-E665AE1BCFCD}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="53">
   <si>
     <t>&lt;prolog&gt;</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>asdasdsadsadasdasdasdsad + 5</t>
+  </si>
+  <si>
+    <t>print</t>
+  </si>
+  <si>
+    <t>&lt;print_params&gt;</t>
   </si>
 </sst>
 </file>
@@ -200,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,12 +294,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,9 +507,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,22 +537,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -581,13 +578,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>41114</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>109883</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -887,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,405 +900,405 @@
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="29" t="s">
+      <c r="J6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="29" t="s">
+      <c r="L6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="29"/>
+      <c r="M6" s="28"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
       <c r="P18" s="1" t="s">
         <v>50</v>
       </c>
@@ -1310,45 +1307,45 @@
       <c r="A19" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
       <c r="P20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1360,641 +1357,684 @@
       <c r="A21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="I22" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="29" t="s">
+      <c r="I23" s="28" t="s">
         <v>14</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="29" t="s">
+      <c r="K23" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="L23" s="29" t="s">
+      <c r="L23" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="M23" s="29"/>
+      <c r="M23" s="28"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C31" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D31" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B32" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C32" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B33" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C33" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D33" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B34" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B35" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C35" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="29"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B36" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C36" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D36" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B37" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="29"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B39" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B40" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
-    </row>
-    <row r="42" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+    </row>
+    <row r="43" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="29" t="s">
+      <c r="B43" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C43" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="D43" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="29" t="s">
+      <c r="E43" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="29" t="s">
+      <c r="B44" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="C44" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="33"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="17"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="32"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="25"/>
+      <c r="A47" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="17"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="25"/>
+      <c r="A48" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="25"/>
+      <c r="A49" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="27"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A50" s="20"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="24"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="26"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="24"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+      <c r="B54" s="23"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="22"/>
+      <c r="B56" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>